<commit_message>
quick committ to make sure I diddnt forget anythnin
</commit_message>
<xml_diff>
--- a/koboforms/section8.xlsx
+++ b/koboforms/section8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deo/whatsthepointgameinteractive/koboforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6898C3DE-2F2A-0946-8A26-516C481EB645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2CD969-5193-D94E-8071-9ABA7A9D4402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1960" yWindow="-18080" windowWidth="28040" windowHeight="17440" xr2:uid="{05574417-E28B-7A44-8D51-6FA488FA6DA5}"/>
   </bookViews>
@@ -132,7 +132,7 @@
     <t>Does a coin put into insurance yield a larger end of season value if there is a drought?</t>
   </si>
   <si>
-    <t>Discuss if  you want to set up an initial pot of money (perhaps from a donor) so that contributions to savings are topping off a complimentary risk fund to keep it sustainable?r why not is it useful have partial insurance?</t>
+    <t>Discuss if  you want to set up an initial pot of money (perhaps from a donor) so that contributions to savings are topping off a complimentary risk fund to keep it sustainable. Why or why not is it useful have partial insurance?</t>
   </si>
 </sst>
 </file>
@@ -189,11 +189,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,22 +520,22 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="93" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -540,91 +549,91 @@
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">

</xml_diff>